<commit_message>
writing for one year volatility
</commit_message>
<xml_diff>
--- a/new_data/independent_variables_corr.xlsx
+++ b/new_data/independent_variables_corr.xlsx
@@ -25,6 +25,9 @@
     <t>skewness</t>
   </si>
   <si>
+    <t>kurtosis</t>
+  </si>
+  <si>
     <t>amihud</t>
   </si>
   <si>
@@ -41,9 +44,6 @@
   </si>
   <si>
     <t>vol_pre</t>
-  </si>
-  <si>
-    <t>spread</t>
   </si>
   <si>
     <t>open_interest</t>
@@ -489,34 +489,34 @@
         <v>-0.02596062146849555</v>
       </c>
       <c r="C2">
-        <v>0.1462780052424883</v>
+        <v>-0.06792257891305753</v>
       </c>
       <c r="D2">
+        <v>0.127374286705381</v>
+      </c>
+      <c r="E2">
         <v>0.05321439153365063</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>-0.08318205529627655</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.0006222378705329488</v>
       </c>
-      <c r="G2">
-        <v>0.06599200862823383</v>
-      </c>
       <c r="H2">
-        <v>0.1035345244326529</v>
+        <v>0.06599200862823393</v>
       </c>
       <c r="I2">
-        <v>-0.116870910580934</v>
+        <v>0.103534524432653</v>
       </c>
       <c r="J2">
-        <v>0.002342779664640943</v>
+        <v>-0.03230258034257761</v>
       </c>
       <c r="K2">
-        <v>0.0004237881750733184</v>
+        <v>0.0004237881750733119</v>
       </c>
       <c r="L2">
-        <v>0.03978958250218724</v>
+        <v>0.01709731236874505</v>
       </c>
       <c r="M2">
         <v>0.02940419783047241</v>
@@ -525,13 +525,13 @@
         <v>0.06818293347164253</v>
       </c>
       <c r="O2">
-        <v>0.06529255357780049</v>
+        <v>0.06529255357780048</v>
       </c>
       <c r="P2">
         <v>-0.05751957549143164</v>
       </c>
       <c r="Q2">
-        <v>0.087522656006432</v>
+        <v>-0.08590055643659278</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -542,34 +542,34 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>-0.04280670556684497</v>
+        <v>0.5542736591930294</v>
       </c>
       <c r="D3">
+        <v>-0.6722939266465148</v>
+      </c>
+      <c r="E3">
         <v>0.03386044397493845</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>-0.2953946030403048</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.05499020499409717</v>
       </c>
-      <c r="G3">
-        <v>0.02790638201429848</v>
-      </c>
       <c r="H3">
-        <v>-0.09110539113689094</v>
+        <v>0.02790638201429849</v>
       </c>
       <c r="I3">
-        <v>0.3395171495494485</v>
+        <v>-0.09110539113689101</v>
       </c>
       <c r="J3">
-        <v>0.01964447176136204</v>
+        <v>0.1302176689297282</v>
       </c>
       <c r="K3">
         <v>0.1707802744286208</v>
       </c>
       <c r="L3">
-        <v>0.3158401581012941</v>
+        <v>-0.1532407111786153</v>
       </c>
       <c r="M3">
         <v>0.1458546538442759</v>
@@ -578,543 +578,543 @@
         <v>-0.03311648640182245</v>
       </c>
       <c r="O3">
-        <v>-0.0800389979311444</v>
+        <v>-0.08003899793114443</v>
       </c>
       <c r="P3">
-        <v>0.008073658175738685</v>
+        <v>0.00807365817573868</v>
       </c>
       <c r="Q3">
-        <v>-0.08656782928105201</v>
+        <v>0.4504485234429239</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4">
-        <v>0.1462780052424883</v>
+        <v>-0.06792257891305753</v>
       </c>
       <c r="B4">
-        <v>-0.04280670556684497</v>
+        <v>0.5542736591930294</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.3877277882645976</v>
+        <v>-0.1437616467305882</v>
       </c>
       <c r="E4">
-        <v>0.1380590871260519</v>
+        <v>-0.3062468081764679</v>
       </c>
       <c r="F4">
-        <v>0.2189198199916903</v>
+        <v>-0.04166653077789922</v>
       </c>
       <c r="G4">
-        <v>0.08431928838637083</v>
+        <v>0.05489822547336181</v>
       </c>
       <c r="H4">
-        <v>0.0574357112735567</v>
+        <v>0.009047622120908805</v>
       </c>
       <c r="I4">
-        <v>0.1530021471701849</v>
+        <v>0.0001839619085308236</v>
       </c>
       <c r="J4">
-        <v>0.1425384458739433</v>
+        <v>-0.02727926313903536</v>
       </c>
       <c r="K4">
-        <v>0.01383127921772829</v>
+        <v>0.05611398453317493</v>
       </c>
       <c r="L4">
-        <v>-0.04880984775936515</v>
+        <v>-0.07708101245672777</v>
       </c>
       <c r="M4">
-        <v>-0.08593608891507505</v>
+        <v>0.08132041989108033</v>
       </c>
       <c r="N4">
-        <v>-0.006939858605727715</v>
+        <v>0.03899178051332702</v>
       </c>
       <c r="O4">
-        <v>0.03946695525751609</v>
+        <v>0.03341198970895573</v>
       </c>
       <c r="P4">
-        <v>0.01532438873584844</v>
+        <v>-0.05726915727237168</v>
       </c>
       <c r="Q4">
-        <v>0.7216279416436614</v>
+        <v>0.776460853462924</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5">
-        <v>0.05321439153365063</v>
+        <v>0.127374286705381</v>
       </c>
       <c r="B5">
-        <v>0.03386044397493845</v>
+        <v>-0.6722939266465148</v>
       </c>
       <c r="C5">
-        <v>0.3877277882645976</v>
+        <v>-0.1437616467305882</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.6361530941453635</v>
+        <v>0.1856823079631591</v>
       </c>
       <c r="F5">
-        <v>0.7273524752812367</v>
+        <v>0.4981285502204547</v>
       </c>
       <c r="G5">
-        <v>0.1924826375294229</v>
+        <v>0.2419691959994472</v>
       </c>
       <c r="H5">
-        <v>-0.1243879243073078</v>
+        <v>-0.01840164647348858</v>
       </c>
       <c r="I5">
-        <v>0.3224662150534713</v>
+        <v>0.07047187697880532</v>
       </c>
       <c r="J5">
-        <v>0.3001271406597706</v>
+        <v>0.01543339531675838</v>
       </c>
       <c r="K5">
-        <v>-0.1620391039947083</v>
+        <v>-0.1684992734965898</v>
       </c>
       <c r="L5">
-        <v>-0.1584203236665656</v>
+        <v>0.1451000279410709</v>
       </c>
       <c r="M5">
-        <v>-0.1757230374760637</v>
+        <v>-0.1477892538188408</v>
       </c>
       <c r="N5">
-        <v>-0.1967552006936234</v>
+        <v>0.005541542908669071</v>
       </c>
       <c r="O5">
-        <v>-0.1563417380003906</v>
+        <v>0.07435966035994092</v>
       </c>
       <c r="P5">
-        <v>0.2087422891114668</v>
+        <v>0.01523555679275454</v>
       </c>
       <c r="Q5">
-        <v>0.2985838228096743</v>
+        <v>-0.1714106362870355</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6">
-        <v>-0.08318205529627655</v>
+        <v>0.05321439153365063</v>
       </c>
       <c r="B6">
-        <v>-0.2953946030403048</v>
+        <v>0.03386044397493845</v>
       </c>
       <c r="C6">
-        <v>0.1380590871260519</v>
+        <v>-0.3062468081764679</v>
       </c>
       <c r="D6">
+        <v>0.1856823079631591</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>0.6361530941453635</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0.6960005294985676</v>
-      </c>
       <c r="G6">
-        <v>0.1513439541284656</v>
+        <v>0.7273524752812367</v>
       </c>
       <c r="H6">
-        <v>-0.06565636359159344</v>
+        <v>0.192482637529423</v>
       </c>
       <c r="I6">
-        <v>0.03313781196017469</v>
+        <v>-0.1243879243073078</v>
       </c>
       <c r="J6">
-        <v>0.3206868254126831</v>
+        <v>0.534804614702407</v>
       </c>
       <c r="K6">
-        <v>-0.2235866524158559</v>
+        <v>-0.1620391039947083</v>
       </c>
       <c r="L6">
-        <v>-0.1552572394539604</v>
+        <v>0.09664407140331076</v>
       </c>
       <c r="M6">
-        <v>-0.2040893177355899</v>
+        <v>-0.1757230374760637</v>
       </c>
       <c r="N6">
-        <v>-0.1275519774768124</v>
+        <v>-0.1967552006936234</v>
       </c>
       <c r="O6">
-        <v>-0.06967366847444849</v>
+        <v>-0.1563417380003906</v>
       </c>
       <c r="P6">
-        <v>0.1333274923959373</v>
+        <v>0.2087422891114668</v>
       </c>
       <c r="Q6">
-        <v>0.1283191339271187</v>
+        <v>-0.2416223378585217</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7">
-        <v>0.0006222378705329488</v>
+        <v>-0.08318205529627655</v>
       </c>
       <c r="B7">
-        <v>0.05499020499409717</v>
+        <v>-0.2953946030403048</v>
       </c>
       <c r="C7">
-        <v>0.2189198199916903</v>
+        <v>-0.04166653077789922</v>
       </c>
       <c r="D7">
-        <v>0.7273524752812367</v>
+        <v>0.4981285502204547</v>
       </c>
       <c r="E7">
+        <v>0.6361530941453635</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>0.6960005294985676</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>0.1661275482465579</v>
-      </c>
       <c r="H7">
-        <v>-0.0710775469862715</v>
+        <v>0.1513439541284659</v>
       </c>
       <c r="I7">
-        <v>0.248336762780068</v>
+        <v>-0.06565636359159345</v>
       </c>
       <c r="J7">
-        <v>0.3545076085593029</v>
+        <v>0.3349955595730471</v>
       </c>
       <c r="K7">
-        <v>-0.1485959568250405</v>
+        <v>-0.2235866524158559</v>
       </c>
       <c r="L7">
-        <v>-0.03259642882855468</v>
+        <v>0.09111724659046457</v>
       </c>
       <c r="M7">
-        <v>-0.1453291580117486</v>
+        <v>-0.2040893177355899</v>
       </c>
       <c r="N7">
-        <v>-0.1492258848970509</v>
+        <v>-0.1275519774768124</v>
       </c>
       <c r="O7">
-        <v>-0.08916160327741868</v>
+        <v>-0.06967366847444846</v>
       </c>
       <c r="P7">
-        <v>0.1664096994858938</v>
+        <v>0.1333274923959373</v>
       </c>
       <c r="Q7">
-        <v>0.1721458560279948</v>
+        <v>-0.0245743112787816</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8">
-        <v>0.06599200862823383</v>
+        <v>0.0006222378705329488</v>
       </c>
       <c r="B8">
-        <v>0.02790638201429848</v>
+        <v>0.05499020499409717</v>
       </c>
       <c r="C8">
-        <v>0.08431928838637083</v>
+        <v>0.05489822547336181</v>
       </c>
       <c r="D8">
-        <v>0.1924826375294229</v>
+        <v>0.2419691959994472</v>
       </c>
       <c r="E8">
-        <v>0.1513439541284656</v>
+        <v>0.7273524752812367</v>
       </c>
       <c r="F8">
-        <v>0.1661275482465579</v>
+        <v>0.6960005294985676</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0.06114989471099779</v>
+        <v>0.1661275482465582</v>
       </c>
       <c r="I8">
-        <v>0.1126663810074422</v>
+        <v>-0.07107754698627147</v>
       </c>
       <c r="J8">
-        <v>0.310333122503364</v>
+        <v>0.4718195929981553</v>
       </c>
       <c r="K8">
-        <v>-0.08169209694182131</v>
+        <v>-0.1485959568250405</v>
       </c>
       <c r="L8">
-        <v>0.09601870575057497</v>
+        <v>0.1427363978668229</v>
       </c>
       <c r="M8">
-        <v>-0.09386926640037974</v>
+        <v>-0.1453291580117486</v>
       </c>
       <c r="N8">
-        <v>-0.0383880120534641</v>
+        <v>-0.1492258848970509</v>
       </c>
       <c r="O8">
-        <v>-0.006457698279505422</v>
+        <v>-0.08916160327741866</v>
       </c>
       <c r="P8">
-        <v>0.02248182617776139</v>
+        <v>0.1664096994858938</v>
       </c>
       <c r="Q8">
-        <v>0.05202362060457395</v>
+        <v>0.02492257974378143</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9">
-        <v>0.1035345244326529</v>
+        <v>0.06599200862823393</v>
       </c>
       <c r="B9">
-        <v>-0.09110539113689094</v>
+        <v>0.02790638201429849</v>
       </c>
       <c r="C9">
-        <v>0.0574357112735567</v>
+        <v>0.009047622120908805</v>
       </c>
       <c r="D9">
-        <v>-0.1243879243073078</v>
+        <v>-0.01840164647348858</v>
       </c>
       <c r="E9">
-        <v>-0.06565636359159344</v>
+        <v>0.192482637529423</v>
       </c>
       <c r="F9">
-        <v>-0.0710775469862715</v>
+        <v>0.1513439541284659</v>
       </c>
       <c r="G9">
+        <v>0.1661275482465582</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>0.06114989471099779</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>-0.2486594034618883</v>
-      </c>
       <c r="J9">
-        <v>0.05520819522197228</v>
+        <v>0.3317632867883254</v>
       </c>
       <c r="K9">
-        <v>0.1253831701299011</v>
+        <v>-0.08169209694182135</v>
       </c>
       <c r="L9">
-        <v>-0.04262421428263236</v>
+        <v>-0.07902730685905968</v>
       </c>
       <c r="M9">
-        <v>0.1548473616074248</v>
+        <v>-0.09386926640037982</v>
       </c>
       <c r="N9">
-        <v>0.9412385020491506</v>
+        <v>-0.03838801205346403</v>
       </c>
       <c r="O9">
-        <v>0.9435525692865563</v>
+        <v>-0.006457698279505384</v>
       </c>
       <c r="P9">
-        <v>-0.8884624562133477</v>
+        <v>0.02248182617776148</v>
       </c>
       <c r="Q9">
-        <v>-0.245891615883863</v>
+        <v>0.005003817325760232</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10">
-        <v>-0.116870910580934</v>
+        <v>0.103534524432653</v>
       </c>
       <c r="B10">
-        <v>0.3395171495494485</v>
+        <v>-0.09110539113689101</v>
       </c>
       <c r="C10">
-        <v>0.1530021471701849</v>
+        <v>0.0001839619085308236</v>
       </c>
       <c r="D10">
-        <v>0.3224662150534713</v>
+        <v>0.07047187697880532</v>
       </c>
       <c r="E10">
-        <v>0.03313781196017469</v>
+        <v>-0.1243879243073078</v>
       </c>
       <c r="F10">
-        <v>0.248336762780068</v>
+        <v>-0.06565636359159345</v>
       </c>
       <c r="G10">
-        <v>0.1126663810074422</v>
+        <v>-0.07107754698627147</v>
       </c>
       <c r="H10">
-        <v>-0.2486594034618883</v>
+        <v>0.06114989471099779</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>0.2249485498296122</v>
+        <v>-0.147619821283394</v>
       </c>
       <c r="K10">
-        <v>0.02144078109232486</v>
+        <v>0.1253831701299011</v>
       </c>
       <c r="L10">
-        <v>0.0228390667649564</v>
+        <v>0.05149792729412004</v>
       </c>
       <c r="M10">
-        <v>-0.02907405538648232</v>
+        <v>0.1548473616074248</v>
       </c>
       <c r="N10">
-        <v>-0.2606051297657284</v>
+        <v>0.9412385020491509</v>
       </c>
       <c r="O10">
-        <v>-0.2132281218835225</v>
+        <v>0.9435525692865563</v>
       </c>
       <c r="P10">
-        <v>0.2371641736059175</v>
+        <v>-0.8884624562133482</v>
       </c>
       <c r="Q10">
-        <v>0.1371536004069459</v>
+        <v>-0.1196685263880993</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11">
-        <v>0.002342779664640943</v>
+        <v>-0.03230258034257761</v>
       </c>
       <c r="B11">
-        <v>0.01964447176136204</v>
+        <v>0.1302176689297282</v>
       </c>
       <c r="C11">
-        <v>0.1425384458739433</v>
+        <v>-0.02727926313903536</v>
       </c>
       <c r="D11">
-        <v>0.3001271406597706</v>
+        <v>0.01543339531675838</v>
       </c>
       <c r="E11">
-        <v>0.3206868254126831</v>
+        <v>0.534804614702407</v>
       </c>
       <c r="F11">
-        <v>0.3545076085593029</v>
+        <v>0.3349955595730471</v>
       </c>
       <c r="G11">
-        <v>0.310333122503364</v>
+        <v>0.4718195929981553</v>
       </c>
       <c r="H11">
-        <v>0.05520819522197228</v>
+        <v>0.3317632867883254</v>
       </c>
       <c r="I11">
-        <v>0.2249485498296122</v>
+        <v>-0.147619821283394</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11">
-        <v>-0.09849274412645219</v>
+        <v>-0.07572380681123662</v>
       </c>
       <c r="L11">
-        <v>0.02022609146361288</v>
+        <v>-0.0865813881341323</v>
       </c>
       <c r="M11">
-        <v>-0.08990111866176559</v>
+        <v>-0.1183019606698989</v>
       </c>
       <c r="N11">
-        <v>-0.03048319128836133</v>
+        <v>-0.2105239057076246</v>
       </c>
       <c r="O11">
-        <v>0.2025901023760964</v>
+        <v>-0.1534732785628016</v>
       </c>
       <c r="P11">
-        <v>0.02560269891537116</v>
+        <v>0.1962347078690383</v>
       </c>
       <c r="Q11">
-        <v>0.1132799913690557</v>
+        <v>-0.05377120925591405</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12">
-        <v>0.0004237881750733184</v>
+        <v>0.0004237881750733119</v>
       </c>
       <c r="B12">
         <v>0.1707802744286208</v>
       </c>
       <c r="C12">
-        <v>0.01383127921772829</v>
+        <v>0.05611398453317493</v>
       </c>
       <c r="D12">
+        <v>-0.1684992734965898</v>
+      </c>
+      <c r="E12">
         <v>-0.1620391039947083</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>-0.2235866524158559</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>-0.1485959568250405</v>
       </c>
-      <c r="G12">
-        <v>-0.08169209694182131</v>
-      </c>
       <c r="H12">
+        <v>-0.08169209694182135</v>
+      </c>
+      <c r="I12">
         <v>0.1253831701299011</v>
       </c>
-      <c r="I12">
-        <v>0.02144078109232486</v>
-      </c>
       <c r="J12">
-        <v>-0.09849274412645219</v>
+        <v>-0.07572380681123662</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12">
-        <v>0.161687058361224</v>
+        <v>-0.1217153524375737</v>
       </c>
       <c r="M12">
-        <v>0.3418468343867792</v>
+        <v>0.3418468343867793</v>
       </c>
       <c r="N12">
         <v>0.1895203005331416</v>
       </c>
       <c r="O12">
-        <v>0.139114964121261</v>
+        <v>0.1391149641212611</v>
       </c>
       <c r="P12">
-        <v>-0.1914223894951325</v>
+        <v>-0.1914223894951326</v>
       </c>
       <c r="Q12">
-        <v>-0.007329001967353086</v>
+        <v>0.01963526155135424</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13">
-        <v>0.03978958250218724</v>
+        <v>0.01709731236874505</v>
       </c>
       <c r="B13">
-        <v>0.3158401581012941</v>
+        <v>-0.1532407111786153</v>
       </c>
       <c r="C13">
-        <v>-0.04880984775936515</v>
+        <v>-0.07708101245672777</v>
       </c>
       <c r="D13">
-        <v>-0.1584203236665656</v>
+        <v>0.1451000279410709</v>
       </c>
       <c r="E13">
-        <v>-0.1552572394539604</v>
+        <v>0.09664407140331076</v>
       </c>
       <c r="F13">
-        <v>-0.03259642882855468</v>
+        <v>0.09111724659046457</v>
       </c>
       <c r="G13">
-        <v>0.09601870575057497</v>
+        <v>0.1427363978668229</v>
       </c>
       <c r="H13">
-        <v>-0.04262421428263236</v>
+        <v>-0.07902730685905968</v>
       </c>
       <c r="I13">
-        <v>0.0228390667649564</v>
+        <v>0.05149792729412004</v>
       </c>
       <c r="J13">
-        <v>0.02022609146361288</v>
+        <v>-0.0865813881341323</v>
       </c>
       <c r="K13">
-        <v>0.161687058361224</v>
+        <v>-0.1217153524375737</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
       <c r="M13">
-        <v>0.1051033241854703</v>
+        <v>-0.07560558277854092</v>
       </c>
       <c r="N13">
-        <v>-0.0493520930160861</v>
+        <v>-0.1901587693476353</v>
       </c>
       <c r="O13">
-        <v>-0.04366343423716059</v>
+        <v>-0.1194581433103747</v>
       </c>
       <c r="P13">
-        <v>0.04126480530673298</v>
+        <v>0.3231529086341685</v>
       </c>
       <c r="Q13">
-        <v>-0.028814317629075</v>
+        <v>0.02214667692113197</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1125,49 +1125,49 @@
         <v>0.1458546538442759</v>
       </c>
       <c r="C14">
-        <v>-0.08593608891507505</v>
+        <v>0.08132041989108033</v>
       </c>
       <c r="D14">
+        <v>-0.1477892538188408</v>
+      </c>
+      <c r="E14">
         <v>-0.1757230374760637</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>-0.2040893177355899</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>-0.1453291580117486</v>
       </c>
-      <c r="G14">
-        <v>-0.09386926640037974</v>
-      </c>
       <c r="H14">
+        <v>-0.09386926640037982</v>
+      </c>
+      <c r="I14">
         <v>0.1548473616074248</v>
       </c>
-      <c r="I14">
-        <v>-0.02907405538648232</v>
-      </c>
       <c r="J14">
-        <v>-0.08990111866176559</v>
+        <v>-0.1183019606698989</v>
       </c>
       <c r="K14">
-        <v>0.3418468343867792</v>
+        <v>0.3418468343867793</v>
       </c>
       <c r="L14">
-        <v>0.1051033241854703</v>
+        <v>-0.07560558277854092</v>
       </c>
       <c r="M14">
         <v>1</v>
       </c>
       <c r="N14">
-        <v>0.1990609751905231</v>
+        <v>0.199060975190523</v>
       </c>
       <c r="O14">
-        <v>0.160877544599199</v>
+        <v>0.1608775445991989</v>
       </c>
       <c r="P14">
         <v>-0.1925875752328105</v>
       </c>
       <c r="Q14">
-        <v>-0.106593809563061</v>
+        <v>0.06964651573374943</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1178,37 +1178,37 @@
         <v>-0.03311648640182245</v>
       </c>
       <c r="C15">
-        <v>-0.006939858605727715</v>
+        <v>0.03899178051332702</v>
       </c>
       <c r="D15">
+        <v>0.005541542908669071</v>
+      </c>
+      <c r="E15">
         <v>-0.1967552006936234</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>-0.1275519774768124</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>-0.1492258848970509</v>
       </c>
-      <c r="G15">
-        <v>-0.0383880120534641</v>
-      </c>
       <c r="H15">
-        <v>0.9412385020491506</v>
+        <v>-0.03838801205346403</v>
       </c>
       <c r="I15">
-        <v>-0.2606051297657284</v>
+        <v>0.9412385020491509</v>
       </c>
       <c r="J15">
-        <v>-0.03048319128836133</v>
+        <v>-0.2105239057076246</v>
       </c>
       <c r="K15">
         <v>0.1895203005331416</v>
       </c>
       <c r="L15">
-        <v>-0.0493520930160861</v>
+        <v>-0.1901587693476353</v>
       </c>
       <c r="M15">
-        <v>0.1990609751905231</v>
+        <v>0.199060975190523</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -1220,48 +1220,48 @@
         <v>-0.9828670152480208</v>
       </c>
       <c r="Q15">
-        <v>-0.3194510450390244</v>
+        <v>-0.1058421727562293</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16">
-        <v>0.06529255357780049</v>
+        <v>0.06529255357780048</v>
       </c>
       <c r="B16">
-        <v>-0.0800389979311444</v>
+        <v>-0.08003899793114443</v>
       </c>
       <c r="C16">
-        <v>0.03946695525751609</v>
+        <v>0.03341198970895573</v>
       </c>
       <c r="D16">
+        <v>0.07435966035994092</v>
+      </c>
+      <c r="E16">
         <v>-0.1563417380003906</v>
       </c>
-      <c r="E16">
-        <v>-0.06967366847444849</v>
-      </c>
       <c r="F16">
-        <v>-0.08916160327741868</v>
+        <v>-0.06967366847444846</v>
       </c>
       <c r="G16">
-        <v>-0.006457698279505422</v>
+        <v>-0.08916160327741866</v>
       </c>
       <c r="H16">
+        <v>-0.006457698279505384</v>
+      </c>
+      <c r="I16">
         <v>0.9435525692865563</v>
       </c>
-      <c r="I16">
-        <v>-0.2132281218835225</v>
-      </c>
       <c r="J16">
-        <v>0.2025901023760964</v>
+        <v>-0.1534732785628016</v>
       </c>
       <c r="K16">
-        <v>0.139114964121261</v>
+        <v>0.1391149641212611</v>
       </c>
       <c r="L16">
-        <v>-0.04366343423716059</v>
+        <v>-0.1194581433103747</v>
       </c>
       <c r="M16">
-        <v>0.160877544599199</v>
+        <v>0.1608775445991989</v>
       </c>
       <c r="N16">
         <v>0.9488590992266038</v>
@@ -1273,7 +1273,7 @@
         <v>-0.9326023107477749</v>
       </c>
       <c r="Q16">
-        <v>-0.2456331831213895</v>
+        <v>-0.1049714584497847</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1281,37 +1281,37 @@
         <v>-0.05751957549143164</v>
       </c>
       <c r="B17">
-        <v>0.008073658175738685</v>
+        <v>0.00807365817573868</v>
       </c>
       <c r="C17">
-        <v>0.01532438873584844</v>
+        <v>-0.05726915727237168</v>
       </c>
       <c r="D17">
+        <v>0.01523555679275454</v>
+      </c>
+      <c r="E17">
         <v>0.2087422891114668</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>0.1333274923959373</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>0.1664096994858938</v>
       </c>
-      <c r="G17">
-        <v>0.02248182617776139</v>
-      </c>
       <c r="H17">
-        <v>-0.8884624562133477</v>
+        <v>0.02248182617776148</v>
       </c>
       <c r="I17">
-        <v>0.2371641736059175</v>
+        <v>-0.8884624562133482</v>
       </c>
       <c r="J17">
-        <v>0.02560269891537116</v>
+        <v>0.1962347078690383</v>
       </c>
       <c r="K17">
-        <v>-0.1914223894951325</v>
+        <v>-0.1914223894951326</v>
       </c>
       <c r="L17">
-        <v>0.04126480530673298</v>
+        <v>0.3231529086341685</v>
       </c>
       <c r="M17">
         <v>-0.1925875752328105</v>
@@ -1326,57 +1326,57 @@
         <v>1</v>
       </c>
       <c r="Q17">
-        <v>0.3139778951553645</v>
+        <v>0.1040287804242795</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18">
-        <v>0.087522656006432</v>
+        <v>-0.08590055643659278</v>
       </c>
       <c r="B18">
-        <v>-0.08656782928105201</v>
+        <v>0.4504485234429239</v>
       </c>
       <c r="C18">
-        <v>0.7216279416436614</v>
+        <v>0.776460853462924</v>
       </c>
       <c r="D18">
-        <v>0.2985838228096743</v>
+        <v>-0.1714106362870355</v>
       </c>
       <c r="E18">
-        <v>0.1283191339271187</v>
+        <v>-0.2416223378585217</v>
       </c>
       <c r="F18">
-        <v>0.1721458560279948</v>
+        <v>-0.0245743112787816</v>
       </c>
       <c r="G18">
-        <v>0.05202362060457395</v>
+        <v>0.02492257974378143</v>
       </c>
       <c r="H18">
-        <v>-0.245891615883863</v>
+        <v>0.005003817325760232</v>
       </c>
       <c r="I18">
-        <v>0.1371536004069459</v>
+        <v>-0.1196685263880993</v>
       </c>
       <c r="J18">
-        <v>0.1132799913690557</v>
+        <v>-0.05377120925591405</v>
       </c>
       <c r="K18">
-        <v>-0.007329001967353086</v>
+        <v>0.01963526155135424</v>
       </c>
       <c r="L18">
-        <v>-0.028814317629075</v>
+        <v>0.02214667692113197</v>
       </c>
       <c r="M18">
-        <v>-0.106593809563061</v>
+        <v>0.06964651573374943</v>
       </c>
       <c r="N18">
-        <v>-0.3194510450390244</v>
+        <v>-0.1058421727562293</v>
       </c>
       <c r="O18">
-        <v>-0.2456331831213895</v>
+        <v>-0.1049714584497847</v>
       </c>
       <c r="P18">
-        <v>0.3139778951553645</v>
+        <v>0.1040287804242795</v>
       </c>
       <c r="Q18">
         <v>1</v>

</xml_diff>

<commit_message>
finish paper for midterm
</commit_message>
<xml_diff>
--- a/new_data/independent_variables_corr.xlsx
+++ b/new_data/independent_variables_corr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>log_ret</t>
   </si>
@@ -40,16 +40,13 @@
     <t>time</t>
   </si>
   <si>
-    <t>delta_5</t>
+    <t>delta</t>
   </si>
   <si>
     <t>vol_pre</t>
   </si>
   <si>
     <t>open_interest</t>
-  </si>
-  <si>
-    <t>slope</t>
   </si>
   <si>
     <t>volume</t>
@@ -422,13 +419,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,11 +474,8 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -516,25 +510,22 @@
         <v>0.0004237881750733215</v>
       </c>
       <c r="L2">
-        <v>0.01709731236874504</v>
+        <v>0.0294041978304724</v>
       </c>
       <c r="M2">
-        <v>0.0294041978304724</v>
+        <v>0.06818293347164253</v>
       </c>
       <c r="N2">
-        <v>0.06818293347164253</v>
+        <v>0.06529255357780051</v>
       </c>
       <c r="O2">
-        <v>0.06529255357780051</v>
+        <v>-0.05751957549143165</v>
       </c>
       <c r="P2">
-        <v>-0.05751957549143165</v>
-      </c>
-      <c r="Q2">
         <v>-0.08590055643659276</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>-0.02596062146849555</v>
       </c>
@@ -569,25 +560,22 @@
         <v>0.1707802744286208</v>
       </c>
       <c r="L3">
-        <v>-0.1532407111786153</v>
+        <v>0.1458546538442759</v>
       </c>
       <c r="M3">
-        <v>0.1458546538442759</v>
+        <v>-0.03311648640182245</v>
       </c>
       <c r="N3">
-        <v>-0.03311648640182245</v>
+        <v>-0.0800389979311444</v>
       </c>
       <c r="O3">
-        <v>-0.0800389979311444</v>
+        <v>0.008073658175738687</v>
       </c>
       <c r="P3">
-        <v>0.008073658175738687</v>
-      </c>
-      <c r="Q3">
         <v>0.4504485234429238</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>-0.06792257891305753</v>
       </c>
@@ -622,25 +610,22 @@
         <v>0.05611398453317494</v>
       </c>
       <c r="L4">
-        <v>-0.07708101245672778</v>
+        <v>0.08132041989108033</v>
       </c>
       <c r="M4">
-        <v>0.08132041989108033</v>
+        <v>0.03899178051332702</v>
       </c>
       <c r="N4">
-        <v>0.03899178051332702</v>
+        <v>0.03341198970895572</v>
       </c>
       <c r="O4">
-        <v>0.03341198970895572</v>
+        <v>-0.05726915727237169</v>
       </c>
       <c r="P4">
-        <v>-0.05726915727237169</v>
-      </c>
-      <c r="Q4">
         <v>0.776460853462924</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>0.127374286705381</v>
       </c>
@@ -675,25 +660,22 @@
         <v>-0.1684992734965898</v>
       </c>
       <c r="L5">
-        <v>0.1451000279410709</v>
+        <v>-0.1477892538188408</v>
       </c>
       <c r="M5">
-        <v>-0.1477892538188408</v>
+        <v>0.005541542908669089</v>
       </c>
       <c r="N5">
-        <v>0.005541542908669089</v>
+        <v>0.07435966035994092</v>
       </c>
       <c r="O5">
-        <v>0.07435966035994092</v>
+        <v>0.01523555679275455</v>
       </c>
       <c r="P5">
-        <v>0.01523555679275455</v>
-      </c>
-      <c r="Q5">
         <v>-0.1714106362870355</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>0.05321439153365063</v>
       </c>
@@ -728,25 +710,22 @@
         <v>-0.1620391039947084</v>
       </c>
       <c r="L6">
-        <v>0.09664407140331084</v>
+        <v>-0.1757230374760637</v>
       </c>
       <c r="M6">
-        <v>-0.1757230374760637</v>
+        <v>-0.1967552006936234</v>
       </c>
       <c r="N6">
-        <v>-0.1967552006936234</v>
+        <v>-0.1563417380003906</v>
       </c>
       <c r="O6">
-        <v>-0.1563417380003906</v>
+        <v>0.2087422891114668</v>
       </c>
       <c r="P6">
-        <v>0.2087422891114668</v>
-      </c>
-      <c r="Q6">
         <v>-0.2416223378585217</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>-0.08318205529627655</v>
       </c>
@@ -781,25 +760,22 @@
         <v>-0.2235866524158559</v>
       </c>
       <c r="L7">
-        <v>0.09111724659046455</v>
+        <v>-0.2040893177355899</v>
       </c>
       <c r="M7">
-        <v>-0.2040893177355899</v>
+        <v>-0.1275519774768124</v>
       </c>
       <c r="N7">
-        <v>-0.1275519774768124</v>
+        <v>-0.06967366847444849</v>
       </c>
       <c r="O7">
-        <v>-0.06967366847444849</v>
+        <v>0.1333274923959373</v>
       </c>
       <c r="P7">
-        <v>0.1333274923959373</v>
-      </c>
-      <c r="Q7">
         <v>-0.0245743112787816</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>0.0006222378705329488</v>
       </c>
@@ -834,25 +810,22 @@
         <v>-0.1485959568250405</v>
       </c>
       <c r="L8">
-        <v>0.1427363978668229</v>
+        <v>-0.1453291580117486</v>
       </c>
       <c r="M8">
-        <v>-0.1453291580117486</v>
+        <v>-0.1492258848970509</v>
       </c>
       <c r="N8">
-        <v>-0.1492258848970509</v>
+        <v>-0.08916160327741866</v>
       </c>
       <c r="O8">
-        <v>-0.08916160327741866</v>
+        <v>0.1664096994858938</v>
       </c>
       <c r="P8">
-        <v>0.1664096994858938</v>
-      </c>
-      <c r="Q8">
         <v>0.02492257974378143</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>0.06599200862823384</v>
       </c>
@@ -887,25 +860,22 @@
         <v>-0.08169209694182135</v>
       </c>
       <c r="L9">
-        <v>-0.0790273068590597</v>
+        <v>-0.09386926640037972</v>
       </c>
       <c r="M9">
-        <v>-0.09386926640037972</v>
+        <v>-0.03838801205346407</v>
       </c>
       <c r="N9">
-        <v>-0.03838801205346407</v>
+        <v>-0.006457698279505406</v>
       </c>
       <c r="O9">
-        <v>-0.006457698279505406</v>
+        <v>0.02248182617776142</v>
       </c>
       <c r="P9">
-        <v>0.02248182617776142</v>
-      </c>
-      <c r="Q9">
         <v>0.005003817325760285</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>0.103534524432653</v>
       </c>
@@ -940,25 +910,22 @@
         <v>0.1253831701299011</v>
       </c>
       <c r="L10">
-        <v>0.05149792729412001</v>
+        <v>0.1548473616074248</v>
       </c>
       <c r="M10">
-        <v>0.1548473616074248</v>
+        <v>0.9412385020491509</v>
       </c>
       <c r="N10">
-        <v>0.9412385020491509</v>
+        <v>0.9435525692865563</v>
       </c>
       <c r="O10">
-        <v>0.9435525692865563</v>
+        <v>-0.8884624562133482</v>
       </c>
       <c r="P10">
-        <v>-0.8884624562133482</v>
-      </c>
-      <c r="Q10">
         <v>-0.1196685263880993</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>-0.03228330738912002</v>
       </c>
@@ -993,25 +960,22 @@
         <v>-0.07579524022993889</v>
       </c>
       <c r="L11">
-        <v>-0.08654660860425223</v>
+        <v>-0.1183608305219486</v>
       </c>
       <c r="M11">
-        <v>-0.1183608305219486</v>
+        <v>-0.2105121191046856</v>
       </c>
       <c r="N11">
-        <v>-0.2105121191046856</v>
+        <v>-0.1534401409042605</v>
       </c>
       <c r="O11">
-        <v>-0.1534401409042605</v>
+        <v>0.1962253955792021</v>
       </c>
       <c r="P11">
-        <v>0.1962253955792021</v>
-      </c>
-      <c r="Q11">
         <v>-0.05380739728928473</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>0.0004237881750733215</v>
       </c>
@@ -1046,339 +1010,268 @@
         <v>1</v>
       </c>
       <c r="L12">
-        <v>-0.1217153524375738</v>
+        <v>0.3418468343867793</v>
       </c>
       <c r="M12">
+        <v>0.1895203005331417</v>
+      </c>
+      <c r="N12">
+        <v>0.139114964121261</v>
+      </c>
+      <c r="O12">
+        <v>-0.1914223894951326</v>
+      </c>
+      <c r="P12">
+        <v>0.01963526155135426</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13">
+        <v>0.0294041978304724</v>
+      </c>
+      <c r="B13">
+        <v>0.1458546538442759</v>
+      </c>
+      <c r="C13">
+        <v>0.08132041989108033</v>
+      </c>
+      <c r="D13">
+        <v>-0.1477892538188408</v>
+      </c>
+      <c r="E13">
+        <v>-0.1757230374760637</v>
+      </c>
+      <c r="F13">
+        <v>-0.2040893177355899</v>
+      </c>
+      <c r="G13">
+        <v>-0.1453291580117486</v>
+      </c>
+      <c r="H13">
+        <v>-0.09386926640037972</v>
+      </c>
+      <c r="I13">
+        <v>0.1548473616074248</v>
+      </c>
+      <c r="J13">
+        <v>-0.1183608305219486</v>
+      </c>
+      <c r="K13">
         <v>0.3418468343867793</v>
       </c>
-      <c r="N12">
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0.199060975190523</v>
+      </c>
+      <c r="N13">
+        <v>0.1608775445991989</v>
+      </c>
+      <c r="O13">
+        <v>-0.1925875752328106</v>
+      </c>
+      <c r="P13">
+        <v>0.06964651573374943</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14">
+        <v>0.06818293347164253</v>
+      </c>
+      <c r="B14">
+        <v>-0.03311648640182245</v>
+      </c>
+      <c r="C14">
+        <v>0.03899178051332702</v>
+      </c>
+      <c r="D14">
+        <v>0.005541542908669089</v>
+      </c>
+      <c r="E14">
+        <v>-0.1967552006936234</v>
+      </c>
+      <c r="F14">
+        <v>-0.1275519774768124</v>
+      </c>
+      <c r="G14">
+        <v>-0.1492258848970509</v>
+      </c>
+      <c r="H14">
+        <v>-0.03838801205346407</v>
+      </c>
+      <c r="I14">
+        <v>0.9412385020491509</v>
+      </c>
+      <c r="J14">
+        <v>-0.2105121191046856</v>
+      </c>
+      <c r="K14">
         <v>0.1895203005331417</v>
       </c>
-      <c r="O12">
+      <c r="L14">
+        <v>0.199060975190523</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>0.9488590992266038</v>
+      </c>
+      <c r="O14">
+        <v>-0.982867015248021</v>
+      </c>
+      <c r="P14">
+        <v>-0.1058421727562293</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15">
+        <v>0.06529255357780051</v>
+      </c>
+      <c r="B15">
+        <v>-0.0800389979311444</v>
+      </c>
+      <c r="C15">
+        <v>0.03341198970895572</v>
+      </c>
+      <c r="D15">
+        <v>0.07435966035994092</v>
+      </c>
+      <c r="E15">
+        <v>-0.1563417380003906</v>
+      </c>
+      <c r="F15">
+        <v>-0.06967366847444849</v>
+      </c>
+      <c r="G15">
+        <v>-0.08916160327741866</v>
+      </c>
+      <c r="H15">
+        <v>-0.006457698279505406</v>
+      </c>
+      <c r="I15">
+        <v>0.9435525692865563</v>
+      </c>
+      <c r="J15">
+        <v>-0.1534401409042605</v>
+      </c>
+      <c r="K15">
         <v>0.139114964121261</v>
       </c>
-      <c r="P12">
+      <c r="L15">
+        <v>0.1608775445991989</v>
+      </c>
+      <c r="M15">
+        <v>0.9488590992266038</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>-0.9326023107477749</v>
+      </c>
+      <c r="P15">
+        <v>-0.1049714584497847</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16">
+        <v>-0.05751957549143165</v>
+      </c>
+      <c r="B16">
+        <v>0.008073658175738687</v>
+      </c>
+      <c r="C16">
+        <v>-0.05726915727237169</v>
+      </c>
+      <c r="D16">
+        <v>0.01523555679275455</v>
+      </c>
+      <c r="E16">
+        <v>0.2087422891114668</v>
+      </c>
+      <c r="F16">
+        <v>0.1333274923959373</v>
+      </c>
+      <c r="G16">
+        <v>0.1664096994858938</v>
+      </c>
+      <c r="H16">
+        <v>0.02248182617776142</v>
+      </c>
+      <c r="I16">
+        <v>-0.8884624562133482</v>
+      </c>
+      <c r="J16">
+        <v>0.1962253955792021</v>
+      </c>
+      <c r="K16">
         <v>-0.1914223894951326</v>
       </c>
-      <c r="Q12">
+      <c r="L16">
+        <v>-0.1925875752328106</v>
+      </c>
+      <c r="M16">
+        <v>-0.982867015248021</v>
+      </c>
+      <c r="N16">
+        <v>-0.9326023107477749</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>0.1040287804242795</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17">
+        <v>-0.08590055643659276</v>
+      </c>
+      <c r="B17">
+        <v>0.4504485234429238</v>
+      </c>
+      <c r="C17">
+        <v>0.776460853462924</v>
+      </c>
+      <c r="D17">
+        <v>-0.1714106362870355</v>
+      </c>
+      <c r="E17">
+        <v>-0.2416223378585217</v>
+      </c>
+      <c r="F17">
+        <v>-0.0245743112787816</v>
+      </c>
+      <c r="G17">
+        <v>0.02492257974378143</v>
+      </c>
+      <c r="H17">
+        <v>0.005003817325760285</v>
+      </c>
+      <c r="I17">
+        <v>-0.1196685263880993</v>
+      </c>
+      <c r="J17">
+        <v>-0.05380739728928473</v>
+      </c>
+      <c r="K17">
         <v>0.01963526155135426</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13">
-        <v>0.01709731236874504</v>
-      </c>
-      <c r="B13">
-        <v>-0.1532407111786153</v>
-      </c>
-      <c r="C13">
-        <v>-0.07708101245672778</v>
-      </c>
-      <c r="D13">
-        <v>0.1451000279410709</v>
-      </c>
-      <c r="E13">
-        <v>0.09664407140331084</v>
-      </c>
-      <c r="F13">
-        <v>0.09111724659046455</v>
-      </c>
-      <c r="G13">
-        <v>0.1427363978668229</v>
-      </c>
-      <c r="H13">
-        <v>-0.0790273068590597</v>
-      </c>
-      <c r="I13">
-        <v>0.05149792729412001</v>
-      </c>
-      <c r="J13">
-        <v>-0.08654660860425223</v>
-      </c>
-      <c r="K13">
-        <v>-0.1217153524375738</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-      <c r="M13">
-        <v>-0.07560558277854094</v>
-      </c>
-      <c r="N13">
-        <v>-0.1901587693476354</v>
-      </c>
-      <c r="O13">
-        <v>-0.1194581433103747</v>
-      </c>
-      <c r="P13">
-        <v>0.3231529086341685</v>
-      </c>
-      <c r="Q13">
-        <v>0.02214667692113198</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14">
-        <v>0.0294041978304724</v>
-      </c>
-      <c r="B14">
-        <v>0.1458546538442759</v>
-      </c>
-      <c r="C14">
-        <v>0.08132041989108033</v>
-      </c>
-      <c r="D14">
-        <v>-0.1477892538188408</v>
-      </c>
-      <c r="E14">
-        <v>-0.1757230374760637</v>
-      </c>
-      <c r="F14">
-        <v>-0.2040893177355899</v>
-      </c>
-      <c r="G14">
-        <v>-0.1453291580117486</v>
-      </c>
-      <c r="H14">
-        <v>-0.09386926640037972</v>
-      </c>
-      <c r="I14">
-        <v>0.1548473616074248</v>
-      </c>
-      <c r="J14">
-        <v>-0.1183608305219486</v>
-      </c>
-      <c r="K14">
-        <v>0.3418468343867793</v>
-      </c>
-      <c r="L14">
-        <v>-0.07560558277854094</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14">
-        <v>0.199060975190523</v>
-      </c>
-      <c r="O14">
-        <v>0.1608775445991989</v>
-      </c>
-      <c r="P14">
-        <v>-0.1925875752328106</v>
-      </c>
-      <c r="Q14">
+      <c r="L17">
         <v>0.06964651573374943</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15">
-        <v>0.06818293347164253</v>
-      </c>
-      <c r="B15">
-        <v>-0.03311648640182245</v>
-      </c>
-      <c r="C15">
-        <v>0.03899178051332702</v>
-      </c>
-      <c r="D15">
-        <v>0.005541542908669089</v>
-      </c>
-      <c r="E15">
-        <v>-0.1967552006936234</v>
-      </c>
-      <c r="F15">
-        <v>-0.1275519774768124</v>
-      </c>
-      <c r="G15">
-        <v>-0.1492258848970509</v>
-      </c>
-      <c r="H15">
-        <v>-0.03838801205346407</v>
-      </c>
-      <c r="I15">
-        <v>0.9412385020491509</v>
-      </c>
-      <c r="J15">
-        <v>-0.2105121191046856</v>
-      </c>
-      <c r="K15">
-        <v>0.1895203005331417</v>
-      </c>
-      <c r="L15">
-        <v>-0.1901587693476354</v>
-      </c>
-      <c r="M15">
-        <v>0.199060975190523</v>
-      </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
-      <c r="O15">
-        <v>0.9488590992266038</v>
-      </c>
-      <c r="P15">
-        <v>-0.982867015248021</v>
-      </c>
-      <c r="Q15">
+      <c r="M17">
         <v>-0.1058421727562293</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16">
-        <v>0.06529255357780051</v>
-      </c>
-      <c r="B16">
-        <v>-0.0800389979311444</v>
-      </c>
-      <c r="C16">
-        <v>0.03341198970895572</v>
-      </c>
-      <c r="D16">
-        <v>0.07435966035994092</v>
-      </c>
-      <c r="E16">
-        <v>-0.1563417380003906</v>
-      </c>
-      <c r="F16">
-        <v>-0.06967366847444849</v>
-      </c>
-      <c r="G16">
-        <v>-0.08916160327741866</v>
-      </c>
-      <c r="H16">
-        <v>-0.006457698279505406</v>
-      </c>
-      <c r="I16">
-        <v>0.9435525692865563</v>
-      </c>
-      <c r="J16">
-        <v>-0.1534401409042605</v>
-      </c>
-      <c r="K16">
-        <v>0.139114964121261</v>
-      </c>
-      <c r="L16">
-        <v>-0.1194581433103747</v>
-      </c>
-      <c r="M16">
-        <v>0.1608775445991989</v>
-      </c>
-      <c r="N16">
-        <v>0.9488590992266038</v>
-      </c>
-      <c r="O16">
-        <v>1</v>
-      </c>
-      <c r="P16">
-        <v>-0.9326023107477749</v>
-      </c>
-      <c r="Q16">
+      <c r="N17">
         <v>-0.1049714584497847</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17">
-        <v>-0.05751957549143165</v>
-      </c>
-      <c r="B17">
-        <v>0.008073658175738687</v>
-      </c>
-      <c r="C17">
-        <v>-0.05726915727237169</v>
-      </c>
-      <c r="D17">
-        <v>0.01523555679275455</v>
-      </c>
-      <c r="E17">
-        <v>0.2087422891114668</v>
-      </c>
-      <c r="F17">
-        <v>0.1333274923959373</v>
-      </c>
-      <c r="G17">
-        <v>0.1664096994858938</v>
-      </c>
-      <c r="H17">
-        <v>0.02248182617776142</v>
-      </c>
-      <c r="I17">
-        <v>-0.8884624562133482</v>
-      </c>
-      <c r="J17">
-        <v>0.1962253955792021</v>
-      </c>
-      <c r="K17">
-        <v>-0.1914223894951326</v>
-      </c>
-      <c r="L17">
-        <v>0.3231529086341685</v>
-      </c>
-      <c r="M17">
-        <v>-0.1925875752328106</v>
-      </c>
-      <c r="N17">
-        <v>-0.982867015248021</v>
-      </c>
       <c r="O17">
-        <v>-0.9326023107477749</v>
+        <v>0.1040287804242795</v>
       </c>
       <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>0.1040287804242795</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18">
-        <v>-0.08590055643659276</v>
-      </c>
-      <c r="B18">
-        <v>0.4504485234429238</v>
-      </c>
-      <c r="C18">
-        <v>0.776460853462924</v>
-      </c>
-      <c r="D18">
-        <v>-0.1714106362870355</v>
-      </c>
-      <c r="E18">
-        <v>-0.2416223378585217</v>
-      </c>
-      <c r="F18">
-        <v>-0.0245743112787816</v>
-      </c>
-      <c r="G18">
-        <v>0.02492257974378143</v>
-      </c>
-      <c r="H18">
-        <v>0.005003817325760285</v>
-      </c>
-      <c r="I18">
-        <v>-0.1196685263880993</v>
-      </c>
-      <c r="J18">
-        <v>-0.05380739728928473</v>
-      </c>
-      <c r="K18">
-        <v>0.01963526155135426</v>
-      </c>
-      <c r="L18">
-        <v>0.02214667692113198</v>
-      </c>
-      <c r="M18">
-        <v>0.06964651573374943</v>
-      </c>
-      <c r="N18">
-        <v>-0.1058421727562293</v>
-      </c>
-      <c r="O18">
-        <v>-0.1049714584497847</v>
-      </c>
-      <c r="P18">
-        <v>0.1040287804242795</v>
-      </c>
-      <c r="Q18">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
try different regression subsamples
</commit_message>
<xml_diff>
--- a/new_data/independent_variables_corr.xlsx
+++ b/new_data/independent_variables_corr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>log_ret</t>
   </si>
@@ -419,859 +419,907 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:17">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>-0.02596062146849555</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>-0.06792257891305753</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.127374286705381</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.05321439153365063</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>-0.08318205529627655</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.0006222378705329488</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.06599200862823384</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.103534524432653</v>
       </c>
-      <c r="J2">
-        <v>-0.03228330738912002</v>
-      </c>
       <c r="K2">
-        <v>0.0004237881750733215</v>
+        <v>-0.03228330738911999</v>
       </c>
       <c r="L2">
+        <v>0.0004237881750733334</v>
+      </c>
+      <c r="M2">
         <v>0.0294041978304724</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.06818293347164253</v>
       </c>
-      <c r="N2">
-        <v>0.06529255357780051</v>
-      </c>
       <c r="O2">
-        <v>-0.05751957549143165</v>
+        <v>0.06529255357780046</v>
       </c>
       <c r="P2">
+        <v>-0.05751957549143166</v>
+      </c>
+      <c r="Q2">
         <v>-0.08590055643659276</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3">
+    <row r="3" spans="1:17">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>-0.02596062146849555</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>0.5542736591930294</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>-0.6722939266465148</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.03386044397493845</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>-0.2953946030403048</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.05499020499409717</v>
       </c>
-      <c r="H3">
-        <v>0.02790638201429849</v>
-      </c>
       <c r="I3">
+        <v>0.02790638201429851</v>
+      </c>
+      <c r="J3">
         <v>-0.09110539113689101</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.1300584009995379</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.1707802744286208</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.1458546538442759</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>-0.03311648640182245</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>-0.0800389979311444</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.008073658175738687</v>
       </c>
-      <c r="P3">
-        <v>0.4504485234429238</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4">
+      <c r="Q3">
+        <v>0.450448523442924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>-0.06792257891305753</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.5542736591930294</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>-0.1437616467305882</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>-0.3062468081764679</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>-0.04166653077789922</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.05489822547336181</v>
       </c>
-      <c r="H4">
-        <v>0.009047622120908885</v>
-      </c>
       <c r="I4">
-        <v>0.0001839619085307912</v>
+        <v>0.009047622120908877</v>
       </c>
       <c r="J4">
+        <v>0.0001839619085307989</v>
+      </c>
+      <c r="K4">
         <v>-0.02740124039743167</v>
       </c>
-      <c r="K4">
-        <v>0.05611398453317494</v>
-      </c>
       <c r="L4">
-        <v>0.08132041989108033</v>
+        <v>0.05611398453317495</v>
       </c>
       <c r="M4">
-        <v>0.03899178051332702</v>
+        <v>0.0813204198910803</v>
       </c>
       <c r="N4">
-        <v>0.03341198970895572</v>
+        <v>0.03899178051332701</v>
       </c>
       <c r="O4">
+        <v>0.03341198970895574</v>
+      </c>
+      <c r="P4">
         <v>-0.05726915727237169</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0.776460853462924</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5">
+    <row r="5" spans="1:17">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>0.127374286705381</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>-0.6722939266465148</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>-0.1437616467305882</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>0.1856823079631591</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.4981285502204547</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.2419691959994472</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>-0.01840164647348858</v>
       </c>
-      <c r="I5">
-        <v>0.07047187697880535</v>
-      </c>
       <c r="J5">
-        <v>0.01541216307019381</v>
+        <v>0.07047187697880533</v>
       </c>
       <c r="K5">
+        <v>0.01541216307019379</v>
+      </c>
+      <c r="L5">
         <v>-0.1684992734965898</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>-0.1477892538188408</v>
       </c>
-      <c r="M5">
-        <v>0.005541542908669089</v>
-      </c>
       <c r="N5">
+        <v>0.005541542908669084</v>
+      </c>
+      <c r="O5">
         <v>0.07435966035994092</v>
       </c>
-      <c r="O5">
-        <v>0.01523555679275455</v>
-      </c>
       <c r="P5">
+        <v>0.01523555679275453</v>
+      </c>
+      <c r="Q5">
         <v>-0.1714106362870355</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6">
+    <row r="6" spans="1:17">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>0.05321439153365063</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.03386044397493845</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>-0.3062468081764679</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.1856823079631591</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
       <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>0.6361530941453635</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.7273524752812367</v>
       </c>
-      <c r="H6">
-        <v>0.1924826375294229</v>
-      </c>
       <c r="I6">
+        <v>0.192482637529423</v>
+      </c>
+      <c r="J6">
         <v>-0.1243879243073078</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.5347726330935234</v>
       </c>
-      <c r="K6">
-        <v>-0.1620391039947084</v>
-      </c>
       <c r="L6">
+        <v>-0.1620391039947083</v>
+      </c>
+      <c r="M6">
         <v>-0.1757230374760637</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>-0.1967552006936234</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>-0.1563417380003906</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.2087422891114668</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>-0.2416223378585217</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7">
+    <row r="7" spans="1:17">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>-0.08318205529627655</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>-0.2953946030403048</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>-0.04166653077789922</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.4981285502204547</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.6361530941453635</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
       <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>0.6960005294985676</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.1513439541284656</v>
       </c>
-      <c r="I7">
-        <v>-0.06565636359159344</v>
-      </c>
       <c r="J7">
+        <v>-0.06565636359159349</v>
+      </c>
+      <c r="K7">
         <v>0.3349831610934758</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>-0.2235866524158559</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>-0.2040893177355899</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>-0.1275519774768124</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>-0.06967366847444849</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>0.1333274923959373</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>-0.0245743112787816</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8">
+    <row r="8" spans="1:17">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <v>0.0006222378705329488</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.05499020499409717</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.05489822547336181</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.2419691959994472</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.7273524752812367</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.6960005294985676</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
       <c r="H8">
-        <v>0.1661275482465578</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>-0.07107754698627149</v>
+        <v>0.1661275482465579</v>
       </c>
       <c r="J8">
+        <v>-0.07107754698627144</v>
+      </c>
+      <c r="K8">
         <v>0.4717540492626066</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>-0.1485959568250405</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>-0.1453291580117486</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>-0.1492258848970509</v>
       </c>
-      <c r="N8">
-        <v>-0.08916160327741866</v>
-      </c>
       <c r="O8">
+        <v>-0.08916160327741865</v>
+      </c>
+      <c r="P8">
         <v>0.1664096994858938</v>
       </c>
-      <c r="P8">
-        <v>0.02492257974378143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9">
+      <c r="Q8">
+        <v>0.02492257974378142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>0.06599200862823384</v>
       </c>
-      <c r="B9">
-        <v>0.02790638201429849</v>
-      </c>
       <c r="C9">
-        <v>0.009047622120908885</v>
+        <v>0.02790638201429851</v>
       </c>
       <c r="D9">
+        <v>0.009047622120908877</v>
+      </c>
+      <c r="E9">
         <v>-0.01840164647348858</v>
       </c>
-      <c r="E9">
-        <v>0.1924826375294229</v>
-      </c>
       <c r="F9">
+        <v>0.192482637529423</v>
+      </c>
+      <c r="G9">
         <v>0.1513439541284656</v>
       </c>
-      <c r="G9">
-        <v>0.1661275482465578</v>
-      </c>
       <c r="H9">
-        <v>1</v>
+        <v>0.1661275482465579</v>
       </c>
       <c r="I9">
-        <v>0.06114989471099781</v>
+        <v>1</v>
       </c>
       <c r="J9">
+        <v>0.06114989471099785</v>
+      </c>
+      <c r="K9">
         <v>0.3320292429978942</v>
       </c>
-      <c r="K9">
-        <v>-0.08169209694182135</v>
-      </c>
       <c r="L9">
-        <v>-0.09386926640037972</v>
+        <v>-0.08169209694182131</v>
       </c>
       <c r="M9">
+        <v>-0.09386926640037974</v>
+      </c>
+      <c r="N9">
         <v>-0.03838801205346407</v>
       </c>
-      <c r="N9">
-        <v>-0.006457698279505406</v>
-      </c>
       <c r="O9">
-        <v>0.02248182617776142</v>
+        <v>-0.00645769827950542</v>
       </c>
       <c r="P9">
+        <v>0.0224818261777614</v>
+      </c>
+      <c r="Q9">
         <v>0.005003817325760285</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10">
+    <row r="10" spans="1:17">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
         <v>0.103534524432653</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>-0.09110539113689101</v>
       </c>
-      <c r="C10">
-        <v>0.0001839619085307912</v>
-      </c>
       <c r="D10">
-        <v>0.07047187697880535</v>
+        <v>0.0001839619085307989</v>
       </c>
       <c r="E10">
+        <v>0.07047187697880533</v>
+      </c>
+      <c r="F10">
         <v>-0.1243879243073078</v>
       </c>
-      <c r="F10">
-        <v>-0.06565636359159344</v>
-      </c>
       <c r="G10">
-        <v>-0.07107754698627149</v>
+        <v>-0.06565636359159349</v>
       </c>
       <c r="H10">
-        <v>0.06114989471099781</v>
+        <v>-0.07107754698627144</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0.06114989471099785</v>
       </c>
       <c r="J10">
-        <v>-0.1475655108299861</v>
+        <v>1</v>
       </c>
       <c r="K10">
+        <v>-0.147565510829986</v>
+      </c>
+      <c r="L10">
         <v>0.1253831701299011</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>0.1548473616074248</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>0.9412385020491509</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>0.9435525692865563</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>-0.8884624562133482</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>-0.1196685263880993</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
-      <c r="A11">
-        <v>-0.03228330738912002</v>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B11">
+        <v>-0.03228330738911999</v>
+      </c>
+      <c r="C11">
         <v>0.1300584009995379</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>-0.02740124039743167</v>
       </c>
-      <c r="D11">
-        <v>0.01541216307019381</v>
-      </c>
       <c r="E11">
+        <v>0.01541216307019379</v>
+      </c>
+      <c r="F11">
         <v>0.5347726330935234</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>0.3349831610934758</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.4717540492626066</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.3320292429978942</v>
       </c>
-      <c r="I11">
-        <v>-0.1475655108299861</v>
-      </c>
       <c r="J11">
-        <v>1</v>
+        <v>-0.147565510829986</v>
       </c>
       <c r="K11">
-        <v>-0.07579524022993889</v>
+        <v>1</v>
       </c>
       <c r="L11">
-        <v>-0.1183608305219486</v>
+        <v>-0.0757952402299389</v>
       </c>
       <c r="M11">
-        <v>-0.2105121191046856</v>
+        <v>-0.1183608305219487</v>
       </c>
       <c r="N11">
+        <v>-0.2105121191046855</v>
+      </c>
+      <c r="O11">
         <v>-0.1534401409042605</v>
       </c>
-      <c r="O11">
-        <v>0.1962253955792021</v>
-      </c>
       <c r="P11">
+        <v>0.196225395579202</v>
+      </c>
+      <c r="Q11">
         <v>-0.05380739728928473</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
-      <c r="A12">
-        <v>0.0004237881750733215</v>
+    <row r="12" spans="1:17">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B12">
+        <v>0.0004237881750733334</v>
+      </c>
+      <c r="C12">
         <v>0.1707802744286208</v>
       </c>
-      <c r="C12">
-        <v>0.05611398453317494</v>
-      </c>
       <c r="D12">
+        <v>0.05611398453317495</v>
+      </c>
+      <c r="E12">
         <v>-0.1684992734965898</v>
       </c>
-      <c r="E12">
-        <v>-0.1620391039947084</v>
-      </c>
       <c r="F12">
+        <v>-0.1620391039947083</v>
+      </c>
+      <c r="G12">
         <v>-0.2235866524158559</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>-0.1485959568250405</v>
       </c>
-      <c r="H12">
-        <v>-0.08169209694182135</v>
-      </c>
       <c r="I12">
+        <v>-0.08169209694182131</v>
+      </c>
+      <c r="J12">
         <v>0.1253831701299011</v>
       </c>
-      <c r="J12">
-        <v>-0.07579524022993889</v>
-      </c>
       <c r="K12">
-        <v>1</v>
+        <v>-0.0757952402299389</v>
       </c>
       <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>0.3418468343867793</v>
       </c>
-      <c r="M12">
-        <v>0.1895203005331417</v>
-      </c>
       <c r="N12">
-        <v>0.139114964121261</v>
+        <v>0.1895203005331416</v>
       </c>
       <c r="O12">
+        <v>0.1391149641212611</v>
+      </c>
+      <c r="P12">
         <v>-0.1914223894951326</v>
       </c>
-      <c r="P12">
-        <v>0.01963526155135426</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13">
+      <c r="Q12">
+        <v>0.01963526155135424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
         <v>0.0294041978304724</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>0.1458546538442759</v>
       </c>
-      <c r="C13">
-        <v>0.08132041989108033</v>
-      </c>
       <c r="D13">
+        <v>0.0813204198910803</v>
+      </c>
+      <c r="E13">
         <v>-0.1477892538188408</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>-0.1757230374760637</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>-0.2040893177355899</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>-0.1453291580117486</v>
       </c>
-      <c r="H13">
-        <v>-0.09386926640037972</v>
-      </c>
       <c r="I13">
+        <v>-0.09386926640037974</v>
+      </c>
+      <c r="J13">
         <v>0.1548473616074248</v>
       </c>
-      <c r="J13">
-        <v>-0.1183608305219486</v>
-      </c>
       <c r="K13">
+        <v>-0.1183608305219487</v>
+      </c>
+      <c r="L13">
         <v>0.3418468343867793</v>
       </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
       <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
         <v>0.199060975190523</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>0.1608775445991989</v>
       </c>
-      <c r="O13">
-        <v>-0.1925875752328106</v>
-      </c>
       <c r="P13">
-        <v>0.06964651573374943</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14">
+        <v>-0.1925875752328105</v>
+      </c>
+      <c r="Q13">
+        <v>0.0696465157337494</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
         <v>0.06818293347164253</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>-0.03311648640182245</v>
       </c>
-      <c r="C14">
-        <v>0.03899178051332702</v>
-      </c>
       <c r="D14">
-        <v>0.005541542908669089</v>
+        <v>0.03899178051332701</v>
       </c>
       <c r="E14">
+        <v>0.005541542908669084</v>
+      </c>
+      <c r="F14">
         <v>-0.1967552006936234</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>-0.1275519774768124</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>-0.1492258848970509</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>-0.03838801205346407</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.9412385020491509</v>
       </c>
-      <c r="J14">
-        <v>-0.2105121191046856</v>
-      </c>
       <c r="K14">
-        <v>0.1895203005331417</v>
+        <v>-0.2105121191046855</v>
       </c>
       <c r="L14">
+        <v>0.1895203005331416</v>
+      </c>
+      <c r="M14">
         <v>0.199060975190523</v>
       </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
       <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
         <v>0.9488590992266038</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>-0.982867015248021</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>-0.1058421727562293</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15">
-        <v>0.06529255357780051</v>
+    <row r="15" spans="1:17">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B15">
+        <v>0.06529255357780046</v>
+      </c>
+      <c r="C15">
         <v>-0.0800389979311444</v>
       </c>
-      <c r="C15">
-        <v>0.03341198970895572</v>
-      </c>
       <c r="D15">
+        <v>0.03341198970895574</v>
+      </c>
+      <c r="E15">
         <v>0.07435966035994092</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>-0.1563417380003906</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>-0.06967366847444849</v>
       </c>
-      <c r="G15">
-        <v>-0.08916160327741866</v>
-      </c>
       <c r="H15">
-        <v>-0.006457698279505406</v>
+        <v>-0.08916160327741865</v>
       </c>
       <c r="I15">
+        <v>-0.00645769827950542</v>
+      </c>
+      <c r="J15">
         <v>0.9435525692865563</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>-0.1534401409042605</v>
       </c>
-      <c r="K15">
-        <v>0.139114964121261</v>
-      </c>
       <c r="L15">
+        <v>0.1391149641212611</v>
+      </c>
+      <c r="M15">
         <v>0.1608775445991989</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>0.9488590992266038</v>
       </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
       <c r="O15">
-        <v>-0.9326023107477749</v>
+        <v>1</v>
       </c>
       <c r="P15">
+        <v>-0.9326023107477747</v>
+      </c>
+      <c r="Q15">
         <v>-0.1049714584497847</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16">
-        <v>-0.05751957549143165</v>
+    <row r="16" spans="1:17">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B16">
+        <v>-0.05751957549143166</v>
+      </c>
+      <c r="C16">
         <v>0.008073658175738687</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>-0.05726915727237169</v>
       </c>
-      <c r="D16">
-        <v>0.01523555679275455</v>
-      </c>
       <c r="E16">
+        <v>0.01523555679275453</v>
+      </c>
+      <c r="F16">
         <v>0.2087422891114668</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>0.1333274923959373</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>0.1664096994858938</v>
       </c>
-      <c r="H16">
-        <v>0.02248182617776142</v>
-      </c>
       <c r="I16">
+        <v>0.0224818261777614</v>
+      </c>
+      <c r="J16">
         <v>-0.8884624562133482</v>
       </c>
-      <c r="J16">
-        <v>0.1962253955792021</v>
-      </c>
       <c r="K16">
+        <v>0.196225395579202</v>
+      </c>
+      <c r="L16">
         <v>-0.1914223894951326</v>
       </c>
-      <c r="L16">
-        <v>-0.1925875752328106</v>
-      </c>
       <c r="M16">
+        <v>-0.1925875752328105</v>
+      </c>
+      <c r="N16">
         <v>-0.982867015248021</v>
       </c>
-      <c r="N16">
-        <v>-0.9326023107477749</v>
-      </c>
       <c r="O16">
-        <v>1</v>
+        <v>-0.9326023107477747</v>
       </c>
       <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
         <v>0.1040287804242795</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
-      <c r="A17">
+    <row r="17" spans="1:17">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
         <v>-0.08590055643659276</v>
       </c>
-      <c r="B17">
-        <v>0.4504485234429238</v>
-      </c>
       <c r="C17">
+        <v>0.450448523442924</v>
+      </c>
+      <c r="D17">
         <v>0.776460853462924</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>-0.1714106362870355</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>-0.2416223378585217</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>-0.0245743112787816</v>
       </c>
-      <c r="G17">
-        <v>0.02492257974378143</v>
-      </c>
       <c r="H17">
+        <v>0.02492257974378142</v>
+      </c>
+      <c r="I17">
         <v>0.005003817325760285</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>-0.1196685263880993</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>-0.05380739728928473</v>
       </c>
-      <c r="K17">
-        <v>0.01963526155135426</v>
-      </c>
       <c r="L17">
-        <v>0.06964651573374943</v>
+        <v>0.01963526155135424</v>
       </c>
       <c r="M17">
+        <v>0.0696465157337494</v>
+      </c>
+      <c r="N17">
         <v>-0.1058421727562293</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>-0.1049714584497847</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>0.1040287804242795</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
writing add robust reg
</commit_message>
<xml_diff>
--- a/new_data/independent_variables_corr.xlsx
+++ b/new_data/independent_variables_corr.xlsx
@@ -498,31 +498,31 @@
         <v>0.0006222378705329488</v>
       </c>
       <c r="H2">
-        <v>0.06599200862823383</v>
+        <v>0.06599200862823394</v>
       </c>
       <c r="I2">
-        <v>0.103534524432653</v>
+        <v>0.1035345244326529</v>
       </c>
       <c r="J2">
-        <v>-0.03228330738911997</v>
+        <v>-0.03228330738911998</v>
       </c>
       <c r="K2">
-        <v>0.0004237881750733144</v>
+        <v>0.0004237881750733173</v>
       </c>
       <c r="L2">
-        <v>0.02940419783047242</v>
+        <v>0.02940419783047241</v>
       </c>
       <c r="M2">
-        <v>0.06818293347164253</v>
+        <v>0.0681829334716425</v>
       </c>
       <c r="N2">
-        <v>0.06529255357780051</v>
+        <v>0.06529255357780049</v>
       </c>
       <c r="O2">
-        <v>-0.05751957549143166</v>
+        <v>-0.05751957549143165</v>
       </c>
       <c r="P2">
-        <v>-0.08590055643659276</v>
+        <v>-0.08590055643659278</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -548,10 +548,10 @@
         <v>0.05499020499409717</v>
       </c>
       <c r="H3">
-        <v>0.02790638201429849</v>
+        <v>0.0279063820142985</v>
       </c>
       <c r="I3">
-        <v>-0.09110539113689098</v>
+        <v>-0.09110539113689102</v>
       </c>
       <c r="J3">
         <v>0.1300584009995379</v>
@@ -563,7 +563,7 @@
         <v>0.1458546538442759</v>
       </c>
       <c r="M3">
-        <v>-0.03311648640182242</v>
+        <v>-0.03311648640182248</v>
       </c>
       <c r="N3">
         <v>-0.0800389979311444</v>
@@ -598,22 +598,22 @@
         <v>0.05489822547336181</v>
       </c>
       <c r="H4">
-        <v>0.009047622120908875</v>
+        <v>0.00904762212090883</v>
       </c>
       <c r="I4">
-        <v>0.0001839619085307967</v>
+        <v>0.0001839619085308085</v>
       </c>
       <c r="J4">
-        <v>-0.0274012403974317</v>
+        <v>-0.02740124039743171</v>
       </c>
       <c r="K4">
         <v>0.05611398453317498</v>
       </c>
       <c r="L4">
-        <v>0.08132041989108033</v>
+        <v>0.08132041989108034</v>
       </c>
       <c r="M4">
-        <v>0.03899178051332701</v>
+        <v>0.03899178051332702</v>
       </c>
       <c r="N4">
         <v>0.03341198970895572</v>
@@ -648,13 +648,13 @@
         <v>0.2419691959994472</v>
       </c>
       <c r="H5">
-        <v>-0.01840164647348858</v>
+        <v>-0.01840164647348859</v>
       </c>
       <c r="I5">
-        <v>0.07047187697880532</v>
+        <v>0.07047187697880535</v>
       </c>
       <c r="J5">
-        <v>0.01541216307019374</v>
+        <v>0.01541216307019378</v>
       </c>
       <c r="K5">
         <v>-0.1684992734965898</v>
@@ -663,10 +663,10 @@
         <v>-0.1477892538188408</v>
       </c>
       <c r="M5">
-        <v>0.005541542908669069</v>
+        <v>0.005541542908669082</v>
       </c>
       <c r="N5">
-        <v>0.0743596603599409</v>
+        <v>0.07435966035994092</v>
       </c>
       <c r="O5">
         <v>0.01523555679275453</v>
@@ -698,13 +698,13 @@
         <v>0.7273524752812367</v>
       </c>
       <c r="H6">
-        <v>0.1924826375294229</v>
+        <v>0.192482637529423</v>
       </c>
       <c r="I6">
-        <v>-0.1243879243073077</v>
+        <v>-0.1243879243073078</v>
       </c>
       <c r="J6">
-        <v>0.5347726330935234</v>
+        <v>0.5347726330935233</v>
       </c>
       <c r="K6">
         <v>-0.1620391039947083</v>
@@ -748,10 +748,10 @@
         <v>0.6960005294985676</v>
       </c>
       <c r="H7">
-        <v>0.1513439541284656</v>
+        <v>0.151343954128466</v>
       </c>
       <c r="I7">
-        <v>-0.06565636359159341</v>
+        <v>-0.06565636359159346</v>
       </c>
       <c r="J7">
         <v>0.3349831610934758</v>
@@ -766,7 +766,7 @@
         <v>-0.1275519774768124</v>
       </c>
       <c r="N7">
-        <v>-0.06967366847444843</v>
+        <v>-0.06967366847444849</v>
       </c>
       <c r="O7">
         <v>0.1333274923959373</v>
@@ -798,10 +798,10 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0.1661275482465578</v>
+        <v>0.1661275482465582</v>
       </c>
       <c r="I8">
-        <v>-0.07107754698627144</v>
+        <v>-0.07107754698627147</v>
       </c>
       <c r="J8">
         <v>0.4717540492626066</v>
@@ -810,13 +810,13 @@
         <v>-0.1485959568250405</v>
       </c>
       <c r="L8">
-        <v>-0.1453291580117486</v>
+        <v>-0.1453291580117487</v>
       </c>
       <c r="M8">
         <v>-0.1492258848970509</v>
       </c>
       <c r="N8">
-        <v>-0.08916160327741865</v>
+        <v>-0.08916160327741868</v>
       </c>
       <c r="O8">
         <v>0.1664096994858938</v>
@@ -827,99 +827,99 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9">
-        <v>0.06599200862823383</v>
+        <v>0.06599200862823394</v>
       </c>
       <c r="B9">
-        <v>0.02790638201429849</v>
+        <v>0.0279063820142985</v>
       </c>
       <c r="C9">
-        <v>0.009047622120908875</v>
+        <v>0.00904762212090883</v>
       </c>
       <c r="D9">
-        <v>-0.01840164647348858</v>
+        <v>-0.01840164647348859</v>
       </c>
       <c r="E9">
-        <v>0.1924826375294229</v>
+        <v>0.192482637529423</v>
       </c>
       <c r="F9">
-        <v>0.1513439541284656</v>
+        <v>0.151343954128466</v>
       </c>
       <c r="G9">
-        <v>0.1661275482465578</v>
+        <v>0.1661275482465582</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9">
-        <v>0.06114989471099785</v>
+        <v>0.06114989471099781</v>
       </c>
       <c r="J9">
         <v>0.3320292429978942</v>
       </c>
       <c r="K9">
-        <v>-0.08169209694182129</v>
+        <v>-0.08169209694182133</v>
       </c>
       <c r="L9">
-        <v>-0.09386926640037974</v>
+        <v>-0.09386926640037981</v>
       </c>
       <c r="M9">
-        <v>-0.03838801205346411</v>
+        <v>-0.03838801205346404</v>
       </c>
       <c r="N9">
-        <v>-0.00645769827950542</v>
+        <v>-0.006457698279505409</v>
       </c>
       <c r="O9">
-        <v>0.02248182617776139</v>
+        <v>0.02248182617776144</v>
       </c>
       <c r="P9">
-        <v>0.00500381732576029</v>
+        <v>0.005003817325760233</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10">
-        <v>0.103534524432653</v>
+        <v>0.1035345244326529</v>
       </c>
       <c r="B10">
-        <v>-0.09110539113689098</v>
+        <v>-0.09110539113689102</v>
       </c>
       <c r="C10">
-        <v>0.0001839619085307967</v>
+        <v>0.0001839619085308085</v>
       </c>
       <c r="D10">
-        <v>0.07047187697880532</v>
+        <v>0.07047187697880535</v>
       </c>
       <c r="E10">
-        <v>-0.1243879243073077</v>
+        <v>-0.1243879243073078</v>
       </c>
       <c r="F10">
-        <v>-0.06565636359159341</v>
+        <v>-0.06565636359159346</v>
       </c>
       <c r="G10">
-        <v>-0.07107754698627144</v>
+        <v>-0.07107754698627147</v>
       </c>
       <c r="H10">
-        <v>0.06114989471099785</v>
+        <v>0.06114989471099781</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>-0.147565510829986</v>
+        <v>-0.1475655108299861</v>
       </c>
       <c r="K10">
-        <v>0.125383170129901</v>
+        <v>0.1253831701299011</v>
       </c>
       <c r="L10">
         <v>0.1548473616074248</v>
       </c>
       <c r="M10">
-        <v>0.9412385020491507</v>
+        <v>0.9412385020491509</v>
       </c>
       <c r="N10">
-        <v>0.9435525692865561</v>
+        <v>0.9435525692865565</v>
       </c>
       <c r="O10">
-        <v>-0.8884624562133479</v>
+        <v>-0.8884624562133482</v>
       </c>
       <c r="P10">
         <v>-0.1196685263880993</v>
@@ -927,19 +927,19 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11">
-        <v>-0.03228330738911997</v>
+        <v>-0.03228330738911998</v>
       </c>
       <c r="B11">
         <v>0.1300584009995379</v>
       </c>
       <c r="C11">
-        <v>-0.0274012403974317</v>
+        <v>-0.02740124039743171</v>
       </c>
       <c r="D11">
-        <v>0.01541216307019374</v>
+        <v>0.01541216307019378</v>
       </c>
       <c r="E11">
-        <v>0.5347726330935234</v>
+        <v>0.5347726330935233</v>
       </c>
       <c r="F11">
         <v>0.3349831610934758</v>
@@ -951,7 +951,7 @@
         <v>0.3320292429978942</v>
       </c>
       <c r="I11">
-        <v>-0.147565510829986</v>
+        <v>-0.1475655108299861</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12">
-        <v>0.0004237881750733144</v>
+        <v>0.0004237881750733173</v>
       </c>
       <c r="B12">
         <v>0.1707802744286208</v>
@@ -998,10 +998,10 @@
         <v>-0.1485959568250405</v>
       </c>
       <c r="H12">
-        <v>-0.08169209694182129</v>
+        <v>-0.08169209694182133</v>
       </c>
       <c r="I12">
-        <v>0.125383170129901</v>
+        <v>0.1253831701299011</v>
       </c>
       <c r="J12">
         <v>-0.07579524022993887</v>
@@ -1013,7 +1013,7 @@
         <v>0.3418468343867792</v>
       </c>
       <c r="M12">
-        <v>0.1895203005331417</v>
+        <v>0.1895203005331416</v>
       </c>
       <c r="N12">
         <v>0.139114964121261</v>
@@ -1022,18 +1022,18 @@
         <v>-0.1914223894951325</v>
       </c>
       <c r="P12">
-        <v>0.01963526155135426</v>
+        <v>0.01963526155135424</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13">
-        <v>0.02940419783047242</v>
+        <v>0.02940419783047241</v>
       </c>
       <c r="B13">
         <v>0.1458546538442759</v>
       </c>
       <c r="C13">
-        <v>0.08132041989108033</v>
+        <v>0.08132041989108034</v>
       </c>
       <c r="D13">
         <v>-0.1477892538188408</v>
@@ -1045,10 +1045,10 @@
         <v>-0.2040893177355899</v>
       </c>
       <c r="G13">
-        <v>-0.1453291580117486</v>
+        <v>-0.1453291580117487</v>
       </c>
       <c r="H13">
-        <v>-0.09386926640037974</v>
+        <v>-0.09386926640037981</v>
       </c>
       <c r="I13">
         <v>0.1548473616074248</v>
@@ -1066,27 +1066,27 @@
         <v>0.199060975190523</v>
       </c>
       <c r="N13">
-        <v>0.1608775445991989</v>
+        <v>0.160877544599199</v>
       </c>
       <c r="O13">
         <v>-0.1925875752328105</v>
       </c>
       <c r="P13">
-        <v>0.06964651573374941</v>
+        <v>0.06964651573374943</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14">
-        <v>0.06818293347164253</v>
+        <v>0.0681829334716425</v>
       </c>
       <c r="B14">
-        <v>-0.03311648640182242</v>
+        <v>-0.03311648640182248</v>
       </c>
       <c r="C14">
-        <v>0.03899178051332701</v>
+        <v>0.03899178051332702</v>
       </c>
       <c r="D14">
-        <v>0.005541542908669069</v>
+        <v>0.005541542908669082</v>
       </c>
       <c r="E14">
         <v>-0.1967552006936234</v>
@@ -1098,16 +1098,16 @@
         <v>-0.1492258848970509</v>
       </c>
       <c r="H14">
-        <v>-0.03838801205346411</v>
+        <v>-0.03838801205346404</v>
       </c>
       <c r="I14">
-        <v>0.9412385020491507</v>
+        <v>0.9412385020491509</v>
       </c>
       <c r="J14">
         <v>-0.2105121191046856</v>
       </c>
       <c r="K14">
-        <v>0.1895203005331417</v>
+        <v>0.1895203005331416</v>
       </c>
       <c r="L14">
         <v>0.199060975190523</v>
@@ -1116,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="N14">
-        <v>0.9488590992266043</v>
+        <v>0.9488590992266038</v>
       </c>
       <c r="O14">
         <v>-0.9828670152480208</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15">
-        <v>0.06529255357780051</v>
+        <v>0.06529255357780049</v>
       </c>
       <c r="B15">
         <v>-0.0800389979311444</v>
@@ -1136,22 +1136,22 @@
         <v>0.03341198970895572</v>
       </c>
       <c r="D15">
-        <v>0.0743596603599409</v>
+        <v>0.07435966035994092</v>
       </c>
       <c r="E15">
         <v>-0.1563417380003906</v>
       </c>
       <c r="F15">
-        <v>-0.06967366847444843</v>
+        <v>-0.06967366847444849</v>
       </c>
       <c r="G15">
-        <v>-0.08916160327741865</v>
+        <v>-0.08916160327741868</v>
       </c>
       <c r="H15">
-        <v>-0.00645769827950542</v>
+        <v>-0.006457698279505409</v>
       </c>
       <c r="I15">
-        <v>0.9435525692865561</v>
+        <v>0.9435525692865565</v>
       </c>
       <c r="J15">
         <v>-0.1534401409042605</v>
@@ -1160,10 +1160,10 @@
         <v>0.139114964121261</v>
       </c>
       <c r="L15">
-        <v>0.1608775445991989</v>
+        <v>0.160877544599199</v>
       </c>
       <c r="M15">
-        <v>0.9488590992266043</v>
+        <v>0.9488590992266038</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16">
-        <v>-0.05751957549143166</v>
+        <v>-0.05751957549143165</v>
       </c>
       <c r="B16">
         <v>0.008073658175738685</v>
@@ -1198,10 +1198,10 @@
         <v>0.1664096994858938</v>
       </c>
       <c r="H16">
-        <v>0.02248182617776139</v>
+        <v>0.02248182617776144</v>
       </c>
       <c r="I16">
-        <v>-0.8884624562133479</v>
+        <v>-0.8884624562133482</v>
       </c>
       <c r="J16">
         <v>0.196225395579202</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17">
-        <v>-0.08590055643659276</v>
+        <v>-0.08590055643659278</v>
       </c>
       <c r="B17">
         <v>0.4504485234429239</v>
@@ -1248,7 +1248,7 @@
         <v>0.02492257974378142</v>
       </c>
       <c r="H17">
-        <v>0.00500381732576029</v>
+        <v>0.005003817325760233</v>
       </c>
       <c r="I17">
         <v>-0.1196685263880993</v>
@@ -1257,10 +1257,10 @@
         <v>-0.05380739728928475</v>
       </c>
       <c r="K17">
-        <v>0.01963526155135426</v>
+        <v>0.01963526155135424</v>
       </c>
       <c r="L17">
-        <v>0.06964651573374941</v>
+        <v>0.06964651573374943</v>
       </c>
       <c r="M17">
         <v>-0.1058421727562293</v>

</xml_diff>